<commit_message>
small change to sample parameter for events
</commit_message>
<xml_diff>
--- a/ExcelSheets/Events.xlsx
+++ b/ExcelSheets/Events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zizhensong/programming_projects/EventReminder/ExcelSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FC63574-C86F-4D47-BB53-C5EBCDD4DA78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FADB995-0B5A-334B-BC6B-F1AF11B35A86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9740" yWindow="2860" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{65A49D11-9ED8-4347-BFDA-0C1C8CF167F2}"/>
+    <workbookView xWindow="9740" yWindow="2860" windowWidth="27640" windowHeight="16940" xr2:uid="{65A49D11-9ED8-4347-BFDA-0C1C8CF167F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>keywords</t>
   </si>
@@ -46,12 +46,6 @@
   </si>
   <si>
     <t>San+Diego</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>This Week</t>
   </si>
   <si>
     <t>tech</t>
@@ -64,19 +58,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF6A8759"/>
-      <name val="Menlo"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,9 +87,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,45 +403,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA2DC35-18AE-BB4B-9251-2C1764DF543E}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B02A4C-2A5C-F04D-AFB9-F23AE35C8434}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -468,12 +416,43 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B02A4C-2A5C-F04D-AFB9-F23AE35C8434}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
         <v>25</v>

</xml_diff>

<commit_message>
EventReminderMain: Emailing Capability Implemented
</commit_message>
<xml_diff>
--- a/ExcelSheets/Events.xlsx
+++ b/ExcelSheets/Events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zizhensong/programming_projects/EventReminder/ExcelSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sambe\EventReminder\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FC63574-C86F-4D47-BB53-C5EBCDD4DA78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A33850-BB98-468C-AAC1-DA1252B0855A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9740" yWindow="2860" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{65A49D11-9ED8-4347-BFDA-0C1C8CF167F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{65A49D11-9ED8-4347-BFDA-0C1C8CF167F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,20 +51,20 @@
     <t>date</t>
   </si>
   <si>
-    <t>This Week</t>
-  </si>
-  <si>
     <t>tech</t>
   </si>
   <si>
     <t>within</t>
+  </si>
+  <si>
+    <t>This-Week</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -418,13 +418,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA2DC35-18AE-BB4B-9251-2C1764DF543E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -440,12 +440,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -457,23 +457,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B02A4C-2A5C-F04D-AFB9-F23AE35C8434}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2">
         <v>25</v>

</xml_diff>

<commit_message>
Removed keys and emails for Sam
</commit_message>
<xml_diff>
--- a/ExcelSheets/Events.xlsx
+++ b/ExcelSheets/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sambe\EventReminder\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A33850-BB98-468C-AAC1-DA1252B0855A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC42CABB-5D4A-43A3-B484-100A6D8FB9E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{65A49D11-9ED8-4347-BFDA-0C1C8CF167F2}"/>
   </bookViews>
@@ -42,15 +42,9 @@
     <t>books</t>
   </si>
   <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>San+Diego</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>tech</t>
   </si>
   <si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>This-Week</t>
+  </si>
+  <si>
+    <t>locations</t>
+  </si>
+  <si>
+    <t>dates</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -434,18 +434,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -468,12 +468,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>25</v>

</xml_diff>

<commit_message>
Powershell Scripts for automation
</commit_message>
<xml_diff>
--- a/ExcelSheets/Events.xlsx
+++ b/ExcelSheets/Events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sambe\EventReminder\ExcelSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC42CABB-5D4A-43A3-B484-100A6D8FB9E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB94E2E7-730E-4BA6-BE27-42017E63D6AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{65A49D11-9ED8-4347-BFDA-0C1C8CF167F2}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>books</t>
   </si>
   <si>
-    <t>San+Diego</t>
-  </si>
-  <si>
     <t>tech</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>dates</t>
+  </si>
+  <si>
+    <t>San+Franciso</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -434,18 +434,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -468,12 +468,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>25</v>

</xml_diff>